<commit_message>
Base de datos Relacionada y diagrama terminado
Trabajamos Elmer Chandia
yobany Abrego
</commit_message>
<xml_diff>
--- a/Documentación/Semana 3/normalizacion Terminada.xlsx
+++ b/Documentación/Semana 3/normalizacion Terminada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CLASES\DesarrolloSoftwawe\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CLASES\Desarrolo-de-Software\Documentación\Semana 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C097A5-1F61-4FF5-B388-F6A8E6F315F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CA57AE-C882-48A4-89AB-D00E4CFDD605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
   <si>
     <t>3FN</t>
   </si>
@@ -307,24 +307,12 @@
     <t>FKIdFactura</t>
   </si>
   <si>
-    <t>hoy</t>
-  </si>
-  <si>
     <t>Elmer</t>
   </si>
   <si>
-    <t>Yobany</t>
-  </si>
-  <si>
-    <t>Acetaminofen</t>
-  </si>
-  <si>
     <t>PKIdDetalleFactura</t>
   </si>
   <si>
-    <t>Ibuprofeno</t>
-  </si>
-  <si>
     <t>Forularios</t>
   </si>
   <si>
@@ -350,6 +338,9 @@
   </si>
   <si>
     <t>Categorias de Productos</t>
+  </si>
+  <si>
+    <t>FKEstadoCivil</t>
   </si>
 </sst>
 </file>
@@ -484,13 +475,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -805,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,16 +824,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -853,11 +844,11 @@
       <c r="K3" s="4"/>
       <c r="M3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="Q3" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>102</v>
+      <c r="Q3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -886,11 +877,11 @@
       <c r="O4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>104</v>
+      <c r="Q4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -918,11 +909,11 @@
       <c r="O5" t="s">
         <v>69</v>
       </c>
-      <c r="Q5" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>96</v>
+      <c r="Q5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -950,11 +941,11 @@
       <c r="O6" t="s">
         <v>70</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="R6" s="9" t="s">
-        <v>106</v>
+      <c r="R6" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -982,11 +973,11 @@
       <c r="O7" t="s">
         <v>71</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="R7" s="9" t="s">
-        <v>106</v>
+      <c r="R7" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1002,11 +993,11 @@
       <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="Q8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="R8" s="9" t="s">
-        <v>106</v>
+      <c r="R8" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1022,11 +1013,11 @@
       <c r="I9" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="9" t="s">
-        <v>104</v>
+      <c r="R9" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1042,11 +1033,11 @@
       <c r="I10" t="s">
         <v>32</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="Q10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R10" s="9" t="s">
-        <v>96</v>
+      <c r="R10" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1056,11 +1047,11 @@
       <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="R11" s="9" t="s">
-        <v>96</v>
+      <c r="R11" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1070,38 +1061,41 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="Q12" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>104</v>
+      <c r="Q12" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="R13" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q14" s="8" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q14" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="R14" s="9" t="s">
-        <v>106</v>
+      <c r="R14" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q15" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="R15" s="9" t="s">
-        <v>96</v>
+      <c r="Q15" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1113,11 +1107,11 @@
       <c r="K16" s="4"/>
       <c r="M16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="Q16" s="9" t="s">
+      <c r="Q16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="R16" s="9" t="s">
-        <v>96</v>
+      <c r="R16" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1151,7 +1145,7 @@
         <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
         <v>45</v>
@@ -1269,12 +1263,6 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>11</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
       <c r="E25" t="s">
         <v>81</v>
       </c>
@@ -1283,12 +1271,6 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" t="s">
-        <v>98</v>
-      </c>
       <c r="E26" t="s">
         <v>82</v>
       </c>
@@ -1297,42 +1279,8 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
       <c r="E27" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>